<commit_message>
suport value query in map processor
</commit_message>
<xml_diff>
--- a/test/res/item.xlsx
+++ b/test/res/item.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10608"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\bite\Desktop\github\xlsx-exporter\test\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codetypes/Desktop/Github/xlsx-exporter/test/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74214BCD-FD31-4D39-880C-125109FE0FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A30C0F-C3FA-654C-B353-886F4758FAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-15" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="define" sheetId="2" r:id="rId1"/>
     <sheet name="item" sheetId="1" r:id="rId2"/>
     <sheet name="follow" sheetId="3" r:id="rId3"/>
     <sheet name="map" sheetId="5" r:id="rId4"/>
-    <sheet name="none" sheetId="4" r:id="rId5"/>
+    <sheet name="map_obj" sheetId="7" r:id="rId5"/>
+    <sheet name="map_arr" sheetId="8" r:id="rId6"/>
+    <sheet name="map_field" sheetId="6" r:id="rId7"/>
+    <sheet name="none" sheetId="4" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">define!$A$2:$G$13</definedName>
@@ -109,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="116">
   <si>
     <t>id</t>
   </si>
@@ -457,37 +460,45 @@
     <t>测试22</t>
   </si>
   <si>
-    <t>@map(kind,level)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>@define</t>
     <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>@map(*,kind,level)</t>
+  </si>
+  <si>
+    <t>@map({name,level,kind},kind,level)</t>
+  </si>
+  <si>
+    <t>@map([name,level],kind,level)</t>
+  </si>
+  <si>
+    <t>@map(.comment,kind,level)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -521,13 +532,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -535,7 +546,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -726,14 +737,35 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1040,34 +1072,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.875" customWidth="1"/>
-    <col min="3" max="3" width="24.125" customWidth="1"/>
-    <col min="4" max="4" width="21.125" customWidth="1"/>
-    <col min="5" max="5" width="20.375" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
     <col min="6" max="6" width="8.5" customWidth="1"/>
-    <col min="7" max="7" width="9.625" customWidth="1"/>
-    <col min="8" max="8" width="18.375" style="16" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-    </row>
-    <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
+      <c r="A1" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+    </row>
+    <row r="2" spans="1:8" ht="16">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1093,7 +1125,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="16">
       <c r="A3" s="7" t="s">
         <v>63</v>
       </c>
@@ -1119,7 +1151,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="16">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -1131,7 +1163,7 @@
       <c r="G4" s="8"/>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="16">
       <c r="A5" s="7" t="s">
         <v>17</v>
       </c>
@@ -1157,7 +1189,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="16">
       <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
@@ -1173,7 +1205,7 @@
       <c r="G6" s="8"/>
       <c r="H6" s="9"/>
     </row>
-    <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="16">
       <c r="A7" s="1" t="s">
         <v>65</v>
       </c>
@@ -1193,7 +1225,7 @@
       </c>
       <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="16">
       <c r="A8" s="1" t="s">
         <v>65</v>
       </c>
@@ -1219,7 +1251,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="16">
       <c r="A9" s="1" t="s">
         <v>65</v>
       </c>
@@ -1241,7 +1273,7 @@
       </c>
       <c r="H9" s="18"/>
     </row>
-    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="16">
       <c r="A10" s="1" t="s">
         <v>65</v>
       </c>
@@ -1263,7 +1295,7 @@
       </c>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="16">
       <c r="A11" s="1" t="s">
         <v>65</v>
       </c>
@@ -1285,7 +1317,7 @@
       </c>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="16">
       <c r="A12" s="1" t="s">
         <v>65</v>
       </c>
@@ -1311,7 +1343,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="16">
       <c r="A13" s="1" t="s">
         <v>65</v>
       </c>
@@ -1335,7 +1367,7 @@
       </c>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="16">
       <c r="A14" s="1" t="s">
         <v>65</v>
       </c>
@@ -1359,7 +1391,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="16">
       <c r="A15" s="1" t="s">
         <v>65</v>
       </c>
@@ -1381,7 +1413,7 @@
       </c>
       <c r="H15" s="19"/>
     </row>
-    <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="16">
       <c r="A16" s="1" t="s">
         <v>65</v>
       </c>
@@ -1403,7 +1435,7 @@
       </c>
       <c r="H16" s="19"/>
     </row>
-    <row r="17" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="16">
       <c r="A17" s="1" t="s">
         <v>65</v>
       </c>
@@ -1425,7 +1457,7 @@
       </c>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="16">
       <c r="A18" s="1" t="s">
         <v>65</v>
       </c>
@@ -1466,22 +1498,22 @@
       <selection pane="bottomLeft" sqref="A1:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="6.5" style="10" customWidth="1"/>
-    <col min="2" max="2" width="5.625" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="32.375" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="14.875" style="10" customWidth="1"/>
-    <col min="7" max="7" width="13.125" style="10" customWidth="1"/>
-    <col min="8" max="8" width="11.625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="90.875" style="10" customWidth="1"/>
-    <col min="10" max="10" width="24.375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="90.83203125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="24.33203125" style="10" customWidth="1"/>
     <col min="11" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1513,7 +1545,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1545,7 +1577,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1563,7 +1595,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -1595,7 +1627,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="33" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="34">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1627,7 +1659,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10">
       <c r="A6" s="4">
         <v>10101</v>
       </c>
@@ -1659,7 +1691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10">
       <c r="A7" s="4">
         <v>10102</v>
       </c>
@@ -1691,7 +1723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10">
       <c r="A8" s="4">
         <v>10103</v>
       </c>
@@ -1723,7 +1755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10">
       <c r="A9" s="4">
         <v>10104</v>
       </c>
@@ -1755,7 +1787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10">
       <c r="A10" s="4">
         <v>10105</v>
       </c>
@@ -1787,7 +1819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="A11" s="4">
         <v>10201</v>
       </c>
@@ -1817,7 +1849,7 @@
       </c>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10">
       <c r="A12" s="4">
         <v>10202</v>
       </c>
@@ -1847,7 +1879,7 @@
       </c>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10">
       <c r="A13" s="4">
         <v>10203</v>
       </c>
@@ -1880,7 +1912,7 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="75"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="75"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1896,13 +1928,13 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1913,7 +1945,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="16">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1924,14 +1956,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="16">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="22"/>
     </row>
-    <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="16">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -1942,7 +1974,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1951,7 +1983,7 @@
       </c>
       <c r="C5" s="22"/>
     </row>
-    <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="16">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -1962,7 +1994,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="16">
       <c r="A7" s="4">
         <v>2</v>
       </c>
@@ -1973,7 +2005,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="16">
       <c r="A8" s="4">
         <v>3</v>
       </c>
@@ -1984,7 +2016,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="16">
       <c r="A9" s="4">
         <v>4</v>
       </c>
@@ -1995,14 +2027,14 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="16">
       <c r="A10" s="4">
         <v>5</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="21"/>
     </row>
-    <row r="11" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="16">
       <c r="A11" s="4">
         <v>6</v>
       </c>
@@ -2013,7 +2045,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="16">
       <c r="A12" s="4">
         <v>7</v>
       </c>
@@ -2024,7 +2056,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="16">
       <c r="A13" s="4">
         <v>8</v>
       </c>
@@ -2038,7 +2070,7 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A1:A13">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2049,22 +2081,22 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
     <col min="2" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="11.625" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="27" customFormat="1">
       <c r="A1" s="28" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2081,7 +2113,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="16">
       <c r="A3" s="1" t="s">
         <v>104</v>
       </c>
@@ -2098,7 +2130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="16">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -2109,7 +2141,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="16">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2126,7 +2158,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="16">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2139,7 +2171,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="16">
       <c r="A7" s="25" t="s">
         <v>105</v>
       </c>
@@ -2156,7 +2188,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="16">
       <c r="A8" s="25" t="s">
         <v>105</v>
       </c>
@@ -2173,7 +2205,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="16">
       <c r="A9" s="25" t="s">
         <v>105</v>
       </c>
@@ -2190,7 +2222,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="16">
       <c r="A10" s="25" t="s">
         <v>105</v>
       </c>
@@ -2201,7 +2233,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>110</v>
@@ -2209,6 +2241,348 @@
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
+  <conditionalFormatting sqref="A2:A10">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E541871-473E-3747-A4FF-7005DDAE5E45}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.5" customWidth="1"/>
+    <col min="2" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="27" customFormat="1">
+      <c r="A1" s="28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16">
+      <c r="A3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="16">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16">
+      <c r="A7" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="26">
+        <v>1</v>
+      </c>
+      <c r="D7" s="26">
+        <v>1</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16">
+      <c r="A8" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="26">
+        <v>1</v>
+      </c>
+      <c r="D8" s="26">
+        <v>2</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16">
+      <c r="A9" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="26">
+        <v>2</v>
+      </c>
+      <c r="D9" s="26">
+        <v>1</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16">
+      <c r="A10" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="26">
+        <v>2</v>
+      </c>
+      <c r="D10" s="26">
+        <v>2</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:A10">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D10B9FB-C914-9E4D-9ED5-4AA283A47ADC}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.5" customWidth="1"/>
+    <col min="2" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="27" customFormat="1">
+      <c r="A1" s="28" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16">
+      <c r="A3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="16">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16">
+      <c r="A7" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="26">
+        <v>1</v>
+      </c>
+      <c r="D7" s="26">
+        <v>1</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16">
+      <c r="A8" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="26">
+        <v>1</v>
+      </c>
+      <c r="D8" s="26">
+        <v>2</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16">
+      <c r="A9" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="26">
+        <v>2</v>
+      </c>
+      <c r="D9" s="26">
+        <v>1</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16">
+      <c r="A10" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="26">
+        <v>2</v>
+      </c>
+      <c r="D10" s="26">
+        <v>2</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
   <conditionalFormatting sqref="A2:A10">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
@@ -2216,7 +2590,178 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA9512F-15D7-C04B-B65B-D43362DB2865}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.5" customWidth="1"/>
+    <col min="2" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="27" customFormat="1">
+      <c r="A1" s="28" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16">
+      <c r="A3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="16">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16">
+      <c r="A7" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="26">
+        <v>1</v>
+      </c>
+      <c r="D7" s="26">
+        <v>1</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16">
+      <c r="A8" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="26">
+        <v>1</v>
+      </c>
+      <c r="D8" s="26">
+        <v>2</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16">
+      <c r="A9" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="26">
+        <v>2</v>
+      </c>
+      <c r="D9" s="26">
+        <v>1</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16">
+      <c r="A10" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="26">
+        <v>2</v>
+      </c>
+      <c r="D10" s="26">
+        <v>2</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:A10">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBB972E-C927-480C-A467-3665FD9F033A}">
   <dimension ref="B2"/>
   <sheetViews>
@@ -2224,9 +2769,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:2">
       <c r="B2" s="24" t="s">
         <v>99</v>
       </c>

</xml_diff>

<commit_message>
auto register enum type
</commit_message>
<xml_diff>
--- a/test/res/item.xlsx
+++ b/test/res/item.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codetypes/Desktop/Github/xlsx-exporter/test/res/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\bite\Desktop\github\xlsx-exporter\test\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A30C0F-C3FA-654C-B353-886F4758FAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFD7722-8747-4444-861D-0F5876A3A679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37740" yWindow="435" windowWidth="33675" windowHeight="19725" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="define" sheetId="2" r:id="rId1"/>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="117">
   <si>
     <t>id</t>
   </si>
@@ -401,9 +401,6 @@
     <t>QualityType</t>
   </si>
   <si>
-    <t>bag_type</t>
-  </si>
-  <si>
     <t>物品类型</t>
   </si>
   <si>
@@ -474,31 +471,39 @@
   </si>
   <si>
     <t>@map(.comment,kind,level)</t>
+  </si>
+  <si>
+    <t>ItemType</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BagType</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -532,13 +537,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -546,7 +551,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -741,7 +746,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
   </cellStyles>
   <dxfs count="6">
@@ -1073,23 +1078,23 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.83203125" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.875" customWidth="1"/>
+    <col min="3" max="3" width="24.125" customWidth="1"/>
+    <col min="4" max="4" width="21.125" customWidth="1"/>
+    <col min="5" max="5" width="20.375" customWidth="1"/>
     <col min="6" max="6" width="8.5" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="9.625" customWidth="1"/>
+    <col min="8" max="8" width="18.375" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -1099,7 +1104,7 @@
       <c r="G1" s="30"/>
       <c r="H1" s="30"/>
     </row>
-    <row r="2" spans="1:8" ht="16">
+    <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1125,7 +1130,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16">
+    <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>63</v>
       </c>
@@ -1151,7 +1156,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16">
+    <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -1163,7 +1168,7 @@
       <c r="G4" s="8"/>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="1:8" ht="16">
+    <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>17</v>
       </c>
@@ -1189,7 +1194,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16">
+    <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
@@ -1205,7 +1210,7 @@
       <c r="G6" s="8"/>
       <c r="H6" s="9"/>
     </row>
-    <row r="7" spans="1:8" ht="16">
+    <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>65</v>
       </c>
@@ -1225,7 +1230,7 @@
       </c>
       <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="1:8" ht="16">
+    <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>65</v>
       </c>
@@ -1248,10 +1253,10 @@
         <v>11</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="16">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>65</v>
       </c>
@@ -1273,7 +1278,7 @@
       </c>
       <c r="H9" s="18"/>
     </row>
-    <row r="10" spans="1:8" ht="16">
+    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>65</v>
       </c>
@@ -1295,7 +1300,7 @@
       </c>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" ht="16">
+    <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>65</v>
       </c>
@@ -1317,7 +1322,7 @@
       </c>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:8" ht="16">
+    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>65</v>
       </c>
@@ -1340,10 +1345,10 @@
         <v>11</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="16">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>65</v>
       </c>
@@ -1367,7 +1372,7 @@
       </c>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:8" ht="16">
+    <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>65</v>
       </c>
@@ -1391,7 +1396,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="16">
+    <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>65</v>
       </c>
@@ -1413,7 +1418,7 @@
       </c>
       <c r="H15" s="19"/>
     </row>
-    <row r="16" spans="1:8" ht="16">
+    <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>65</v>
       </c>
@@ -1435,7 +1440,7 @@
       </c>
       <c r="H16" s="19"/>
     </row>
-    <row r="17" spans="1:8" ht="16">
+    <row r="17" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>65</v>
       </c>
@@ -1457,7 +1462,7 @@
       </c>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="1:8" ht="16">
+    <row r="18" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>65</v>
       </c>
@@ -1493,27 +1498,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView showFormulas="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showFormulas="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G5"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6.5" style="10" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="32.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="90.83203125" style="10" customWidth="1"/>
-    <col min="10" max="10" width="24.33203125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="5.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="32.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="14.875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="13.125" style="10" customWidth="1"/>
+    <col min="8" max="8" width="11.625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="90.875" style="10" customWidth="1"/>
+    <col min="10" max="10" width="24.375" style="10" customWidth="1"/>
     <col min="11" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1545,7 +1550,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1559,16 +1564,16 @@
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="11" t="s">
-        <v>7</v>
+      <c r="H2" s="20" t="s">
+        <v>94</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>14</v>
@@ -1577,7 +1582,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1595,7 +1600,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -1627,7 +1632,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="34">
+    <row r="5" spans="1:10" ht="33" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1659,7 +1664,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>10101</v>
       </c>
@@ -1691,7 +1696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>10102</v>
       </c>
@@ -1723,7 +1728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>10103</v>
       </c>
@@ -1755,7 +1760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>10104</v>
       </c>
@@ -1787,7 +1792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>10105</v>
       </c>
@@ -1819,7 +1824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>10201</v>
       </c>
@@ -1849,7 +1854,7 @@
       </c>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>10202</v>
       </c>
@@ -1879,7 +1884,7 @@
       </c>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>10203</v>
       </c>
@@ -1928,13 +1933,13 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16">
+    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1945,7 +1950,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16">
+    <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1956,14 +1961,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16">
+    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="22"/>
     </row>
-    <row r="4" spans="1:3" ht="16">
+    <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -1971,19 +1976,19 @@
         <v>10</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" s="22"/>
     </row>
-    <row r="6" spans="1:3" ht="16">
+    <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -1991,10 +1996,10 @@
         <v>71</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="16">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>2</v>
       </c>
@@ -2002,10 +2007,10 @@
         <v>71</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="16">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>3</v>
       </c>
@@ -2013,10 +2018,10 @@
         <v>71</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="16">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>4</v>
       </c>
@@ -2024,17 +2029,17 @@
         <v>71</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="16">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>5</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="21"/>
     </row>
-    <row r="11" spans="1:3" ht="16">
+    <row r="11" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>6</v>
       </c>
@@ -2042,10 +2047,10 @@
         <v>74</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="16">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>7</v>
       </c>
@@ -2053,10 +2058,10 @@
         <v>74</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="16">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>8</v>
       </c>
@@ -2064,7 +2069,7 @@
         <v>74</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2084,19 +2089,19 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
     <col min="2" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="27" customFormat="1">
+    <row r="1" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="16">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2104,33 +2109,33 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16">
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16">
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -2141,7 +2146,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="16">
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2149,16 +2154,16 @@
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16">
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2171,29 +2176,29 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16">
+    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="C7" s="26">
+        <v>1</v>
+      </c>
+      <c r="D7" s="26">
+        <v>1</v>
+      </c>
+      <c r="E7" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="26">
-        <v>1</v>
-      </c>
-      <c r="D7" s="26">
-        <v>1</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16">
+    </row>
+    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="25" t="s">
         <v>105</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>106</v>
       </c>
       <c r="C8" s="26">
         <v>1</v>
@@ -2202,15 +2207,15 @@
         <v>2</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="16">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="25" t="s">
         <v>105</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>106</v>
       </c>
       <c r="C9" s="26">
         <v>2</v>
@@ -2219,15 +2224,15 @@
         <v>1</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="16">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="25" t="s">
         <v>105</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>106</v>
       </c>
       <c r="C10" s="26">
         <v>2</v>
@@ -2236,7 +2241,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2256,19 +2261,19 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
     <col min="2" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="27" customFormat="1">
+    <row r="1" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="16">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2276,33 +2281,33 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16">
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16">
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -2313,7 +2318,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="16">
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2321,16 +2326,16 @@
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16">
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2343,29 +2348,29 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16">
+    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="C7" s="26">
+        <v>1</v>
+      </c>
+      <c r="D7" s="26">
+        <v>1</v>
+      </c>
+      <c r="E7" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="26">
-        <v>1</v>
-      </c>
-      <c r="D7" s="26">
-        <v>1</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16">
+    </row>
+    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="25" t="s">
         <v>105</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>106</v>
       </c>
       <c r="C8" s="26">
         <v>1</v>
@@ -2374,15 +2379,15 @@
         <v>2</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="16">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="25" t="s">
         <v>105</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>106</v>
       </c>
       <c r="C9" s="26">
         <v>2</v>
@@ -2391,15 +2396,15 @@
         <v>1</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="16">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="25" t="s">
         <v>105</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>106</v>
       </c>
       <c r="C10" s="26">
         <v>2</v>
@@ -2408,12 +2413,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A2:A10">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2427,19 +2433,19 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
     <col min="2" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="27" customFormat="1">
+    <row r="1" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="16">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2447,33 +2453,33 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16">
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16">
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -2484,7 +2490,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="16">
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2492,16 +2498,16 @@
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16">
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2514,29 +2520,29 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16">
+    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="C7" s="26">
+        <v>1</v>
+      </c>
+      <c r="D7" s="26">
+        <v>1</v>
+      </c>
+      <c r="E7" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="26">
-        <v>1</v>
-      </c>
-      <c r="D7" s="26">
-        <v>1</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16">
+    </row>
+    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="25" t="s">
         <v>105</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>106</v>
       </c>
       <c r="C8" s="26">
         <v>1</v>
@@ -2545,15 +2551,15 @@
         <v>2</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="16">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="25" t="s">
         <v>105</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>106</v>
       </c>
       <c r="C9" s="26">
         <v>2</v>
@@ -2562,15 +2568,15 @@
         <v>1</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="16">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="25" t="s">
         <v>105</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>106</v>
       </c>
       <c r="C10" s="26">
         <v>2</v>
@@ -2579,12 +2585,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A2:A10">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2594,23 +2601,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA9512F-15D7-C04B-B65B-D43362DB2865}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
     <col min="2" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="27" customFormat="1">
+    <row r="1" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="16">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2618,33 +2625,33 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16">
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16">
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -2655,7 +2662,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="16">
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2663,16 +2670,16 @@
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16">
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2685,29 +2692,29 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16">
+    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="C7" s="26">
+        <v>1</v>
+      </c>
+      <c r="D7" s="26">
+        <v>1</v>
+      </c>
+      <c r="E7" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="26">
-        <v>1</v>
-      </c>
-      <c r="D7" s="26">
-        <v>1</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16">
+    </row>
+    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="25" t="s">
         <v>105</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>106</v>
       </c>
       <c r="C8" s="26">
         <v>1</v>
@@ -2716,15 +2723,15 @@
         <v>2</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="16">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="25" t="s">
         <v>105</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>106</v>
       </c>
       <c r="C9" s="26">
         <v>2</v>
@@ -2733,15 +2740,15 @@
         <v>1</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="16">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="25" t="s">
         <v>105</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>106</v>
       </c>
       <c r="C10" s="26">
         <v>2</v>
@@ -2750,12 +2757,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A2:A10">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2769,11 +2777,11 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refer type from other field
</commit_message>
<xml_diff>
--- a/test/res/item.xlsx
+++ b/test/res/item.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\bite\Desktop\github\xlsx-exporter\test\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codetypes/Desktop/Github/xlsx-exporter/test/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFD7722-8747-4444-861D-0F5876A3A679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF113DD3-916C-AD43-A82F-1A0D070E0E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37740" yWindow="435" windowWidth="33675" windowHeight="19725" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="define" sheetId="2" r:id="rId1"/>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="119">
   <si>
     <t>id</t>
   </si>
@@ -479,31 +479,37 @@
   <si>
     <t>BagType</t>
     <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>@value_type</t>
+  </si>
+  <si>
+    <t>--</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -537,13 +543,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -551,7 +557,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -746,7 +752,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
   </cellStyles>
   <dxfs count="6">
@@ -1078,21 +1084,21 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.875" customWidth="1"/>
-    <col min="3" max="3" width="24.125" customWidth="1"/>
-    <col min="4" max="4" width="21.125" customWidth="1"/>
-    <col min="5" max="5" width="20.375" customWidth="1"/>
-    <col min="6" max="6" width="8.5" customWidth="1"/>
-    <col min="7" max="7" width="9.625" customWidth="1"/>
-    <col min="8" max="8" width="18.375" style="16" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="29" t="s">
         <v>110</v>
       </c>
@@ -1104,7 +1110,7 @@
       <c r="G1" s="30"/>
       <c r="H1" s="30"/>
     </row>
-    <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="16">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1130,7 +1136,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="16">
       <c r="A3" s="7" t="s">
         <v>63</v>
       </c>
@@ -1147,7 +1153,7 @@
         <v>64</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>12</v>
@@ -1156,7 +1162,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="16">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -1168,7 +1174,7 @@
       <c r="G4" s="8"/>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="16">
       <c r="A5" s="7" t="s">
         <v>17</v>
       </c>
@@ -1194,7 +1200,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="16">
       <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
@@ -1210,7 +1216,7 @@
       <c r="G6" s="8"/>
       <c r="H6" s="9"/>
     </row>
-    <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="16">
       <c r="A7" s="1" t="s">
         <v>65</v>
       </c>
@@ -1230,7 +1236,7 @@
       </c>
       <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="16">
       <c r="A8" s="1" t="s">
         <v>65</v>
       </c>
@@ -1256,7 +1262,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="16">
       <c r="A9" s="1" t="s">
         <v>65</v>
       </c>
@@ -1278,7 +1284,7 @@
       </c>
       <c r="H9" s="18"/>
     </row>
-    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="16">
       <c r="A10" s="1" t="s">
         <v>65</v>
       </c>
@@ -1300,7 +1306,7 @@
       </c>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="16">
       <c r="A11" s="1" t="s">
         <v>65</v>
       </c>
@@ -1322,7 +1328,7 @@
       </c>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="16">
       <c r="A12" s="1" t="s">
         <v>65</v>
       </c>
@@ -1348,7 +1354,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="16">
       <c r="A13" s="1" t="s">
         <v>65</v>
       </c>
@@ -1372,7 +1378,7 @@
       </c>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="16">
       <c r="A14" s="1" t="s">
         <v>65</v>
       </c>
@@ -1396,7 +1402,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="16">
       <c r="A15" s="1" t="s">
         <v>65</v>
       </c>
@@ -1418,7 +1424,7 @@
       </c>
       <c r="H15" s="19"/>
     </row>
-    <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="16">
       <c r="A16" s="1" t="s">
         <v>65</v>
       </c>
@@ -1440,7 +1446,7 @@
       </c>
       <c r="H16" s="19"/>
     </row>
-    <row r="17" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="16">
       <c r="A17" s="1" t="s">
         <v>65</v>
       </c>
@@ -1462,7 +1468,7 @@
       </c>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="16">
       <c r="A18" s="1" t="s">
         <v>65</v>
       </c>
@@ -1498,27 +1504,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showFormulas="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="6.5" style="10" customWidth="1"/>
-    <col min="2" max="2" width="5.625" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="32.375" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="14.875" style="10" customWidth="1"/>
-    <col min="7" max="7" width="13.125" style="10" customWidth="1"/>
-    <col min="8" max="8" width="11.625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="90.875" style="10" customWidth="1"/>
-    <col min="10" max="10" width="24.375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="90.83203125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="24.33203125" style="10" customWidth="1"/>
     <col min="11" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1550,7 +1556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1582,7 +1588,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1600,7 +1606,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -1632,7 +1638,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="33" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="34">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1664,7 +1670,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10">
       <c r="A6" s="4">
         <v>10101</v>
       </c>
@@ -1696,7 +1702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10">
       <c r="A7" s="4">
         <v>10102</v>
       </c>
@@ -1728,7 +1734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10">
       <c r="A8" s="4">
         <v>10103</v>
       </c>
@@ -1760,7 +1766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10">
       <c r="A9" s="4">
         <v>10104</v>
       </c>
@@ -1792,7 +1798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10">
       <c r="A10" s="4">
         <v>10105</v>
       </c>
@@ -1824,7 +1830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="A11" s="4">
         <v>10201</v>
       </c>
@@ -1854,7 +1860,7 @@
       </c>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10">
       <c r="A12" s="4">
         <v>10202</v>
       </c>
@@ -1884,7 +1890,7 @@
       </c>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10">
       <c r="A13" s="4">
         <v>10203</v>
       </c>
@@ -1930,16 +1936,16 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1950,7 +1956,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="16">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1961,14 +1967,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="16">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="22"/>
     </row>
-    <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="16">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -1979,7 +1985,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1988,7 +1994,7 @@
       </c>
       <c r="C5" s="22"/>
     </row>
-    <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="16">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -1999,7 +2005,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="16">
       <c r="A7" s="4">
         <v>2</v>
       </c>
@@ -2010,7 +2016,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="16">
       <c r="A8" s="4">
         <v>3</v>
       </c>
@@ -2021,7 +2027,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="16">
       <c r="A9" s="4">
         <v>4</v>
       </c>
@@ -2032,14 +2038,14 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="16">
       <c r="A10" s="4">
         <v>5</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="21"/>
     </row>
-    <row r="11" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="16">
       <c r="A11" s="4">
         <v>6</v>
       </c>
@@ -2050,7 +2056,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="16">
       <c r="A12" s="4">
         <v>7</v>
       </c>
@@ -2061,7 +2067,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="16">
       <c r="A13" s="4">
         <v>8</v>
       </c>
@@ -2085,25 +2091,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E27B46D-4699-4B1C-B2B1-8A327D06725E}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
     <col min="2" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="11.625" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="27" customFormat="1">
       <c r="A1" s="28" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
+    <row r="2" spans="1:5" ht="16">
+      <c r="A2" s="7" t="s">
+        <v>118</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -2118,7 +2124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="16">
       <c r="A3" s="1" t="s">
         <v>103</v>
       </c>
@@ -2135,7 +2141,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="16">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -2146,7 +2152,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="16">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2163,7 +2169,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="16">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2176,7 +2182,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="16">
       <c r="A7" s="25" t="s">
         <v>104</v>
       </c>
@@ -2193,7 +2199,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="16">
       <c r="A8" s="25" t="s">
         <v>104</v>
       </c>
@@ -2210,7 +2216,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="16">
       <c r="A9" s="25" t="s">
         <v>104</v>
       </c>
@@ -2227,7 +2233,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="16">
       <c r="A10" s="25" t="s">
         <v>104</v>
       </c>
@@ -2261,19 +2267,19 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
     <col min="2" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="11.625" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="27" customFormat="1">
       <c r="A1" s="28" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="16">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2290,7 +2296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="16">
       <c r="A3" s="1" t="s">
         <v>103</v>
       </c>
@@ -2307,7 +2313,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="16">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -2318,7 +2324,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="16">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2335,7 +2341,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="16">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2348,7 +2354,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="16">
       <c r="A7" s="25" t="s">
         <v>104</v>
       </c>
@@ -2365,7 +2371,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="16">
       <c r="A8" s="25" t="s">
         <v>104</v>
       </c>
@@ -2382,7 +2388,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="16">
       <c r="A9" s="25" t="s">
         <v>104</v>
       </c>
@@ -2399,7 +2405,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="16">
       <c r="A10" s="25" t="s">
         <v>104</v>
       </c>
@@ -2433,19 +2439,19 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
     <col min="2" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="11.625" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="27" customFormat="1">
       <c r="A1" s="28" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="16">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2462,7 +2468,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="16">
       <c r="A3" s="1" t="s">
         <v>103</v>
       </c>
@@ -2479,7 +2485,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="16">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -2490,7 +2496,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="16">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2507,7 +2513,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="16">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2520,7 +2526,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="16">
       <c r="A7" s="25" t="s">
         <v>104</v>
       </c>
@@ -2537,7 +2543,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="16">
       <c r="A8" s="25" t="s">
         <v>104</v>
       </c>
@@ -2554,7 +2560,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="16">
       <c r="A9" s="25" t="s">
         <v>104</v>
       </c>
@@ -2571,7 +2577,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="16">
       <c r="A10" s="25" t="s">
         <v>104</v>
       </c>
@@ -2605,19 +2611,19 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
     <col min="2" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="11.625" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="27" customFormat="1">
       <c r="A1" s="28" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="16">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2634,7 +2640,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="16">
       <c r="A3" s="1" t="s">
         <v>103</v>
       </c>
@@ -2651,7 +2657,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="16">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -2662,7 +2668,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="16">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2679,7 +2685,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="16">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2692,7 +2698,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="16">
       <c r="A7" s="25" t="s">
         <v>104</v>
       </c>
@@ -2709,7 +2715,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="16">
       <c r="A8" s="25" t="s">
         <v>104</v>
       </c>
@@ -2726,7 +2732,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="16">
       <c r="A9" s="25" t="s">
         <v>104</v>
       </c>
@@ -2743,7 +2749,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="16">
       <c r="A10" s="25" t="s">
         <v>104</v>
       </c>
@@ -2777,9 +2783,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:2">
       <c r="B2" s="24" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
use '$$' to get row data in expr checker
</commit_message>
<xml_diff>
--- a/test/res/item.xlsx
+++ b/test/res/item.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codetypes/Desktop/Github/xlsx-exporter/test/res/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\bite\Desktop\github\xlsx-exporter\test\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF113DD3-916C-AD43-A82F-1A0D070E0E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E13251E-55ED-44B9-A65E-8ECF2B42EF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30780" yWindow="1335" windowWidth="28395" windowHeight="18750" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="define" sheetId="2" r:id="rId1"/>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="124">
   <si>
     <t>id</t>
   </si>
@@ -408,57 +408,57 @@
   </si>
   <si>
     <t>!@follow(name)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>s</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>kind</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>level</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>int</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>x</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>auto</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>-</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>测试</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>测试1</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>测试2</t>
   </si>
   <si>
     <t>测试21</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>测试22</t>
   </si>
   <si>
     <t>@define</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>@map(*,kind,level)</t>
@@ -474,42 +474,55 @@
   </si>
   <si>
     <t>ItemType</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>BagType</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>@value_type</t>
   </si>
   <si>
     <t>--</t>
+  </si>
+  <si>
+    <t>arr1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>arr2</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>int[]?</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>[1,2]</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>$.length == arr1.length</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -543,13 +556,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -557,7 +570,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -666,93 +679,88 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
   </cellStyles>
   <dxfs count="6">
@@ -1087,30 +1095,30 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.83203125" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.875" customWidth="1"/>
+    <col min="3" max="3" width="24.125" customWidth="1"/>
+    <col min="4" max="4" width="21.125" customWidth="1"/>
+    <col min="5" max="5" width="20.375" customWidth="1"/>
     <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="9.625" customWidth="1"/>
+    <col min="8" max="8" width="18.375" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-    </row>
-    <row r="2" spans="1:8" ht="16">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+    </row>
+    <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1136,7 +1144,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16">
+    <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>63</v>
       </c>
@@ -1162,7 +1170,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16">
+    <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -1174,7 +1182,7 @@
       <c r="G4" s="8"/>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="1:8" ht="16">
+    <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>17</v>
       </c>
@@ -1200,7 +1208,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16">
+    <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
@@ -1216,7 +1224,7 @@
       <c r="G6" s="8"/>
       <c r="H6" s="9"/>
     </row>
-    <row r="7" spans="1:8" ht="16">
+    <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>65</v>
       </c>
@@ -1236,7 +1244,7 @@
       </c>
       <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="1:8" ht="16">
+    <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>65</v>
       </c>
@@ -1262,7 +1270,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16">
+    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>65</v>
       </c>
@@ -1284,7 +1292,7 @@
       </c>
       <c r="H9" s="18"/>
     </row>
-    <row r="10" spans="1:8" ht="16">
+    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>65</v>
       </c>
@@ -1306,7 +1314,7 @@
       </c>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" ht="16">
+    <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>65</v>
       </c>
@@ -1328,7 +1336,7 @@
       </c>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:8" ht="16">
+    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>65</v>
       </c>
@@ -1354,7 +1362,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16">
+    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>65</v>
       </c>
@@ -1378,7 +1386,7 @@
       </c>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:8" ht="16">
+    <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>65</v>
       </c>
@@ -1402,7 +1410,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="16">
+    <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>65</v>
       </c>
@@ -1424,7 +1432,7 @@
       </c>
       <c r="H15" s="19"/>
     </row>
-    <row r="16" spans="1:8" ht="16">
+    <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>65</v>
       </c>
@@ -1446,7 +1454,7 @@
       </c>
       <c r="H16" s="19"/>
     </row>
-    <row r="17" spans="1:8" ht="16">
+    <row r="17" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>65</v>
       </c>
@@ -1468,7 +1476,7 @@
       </c>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="1:8" ht="16">
+    <row r="18" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>65</v>
       </c>
@@ -1494,7 +1502,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
@@ -1509,22 +1517,22 @@
       <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6.5" style="10" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="32.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="90.83203125" style="10" customWidth="1"/>
-    <col min="10" max="10" width="24.33203125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="5.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="32.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="14.875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="13.125" style="10" customWidth="1"/>
+    <col min="8" max="8" width="11.625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="90.875" style="10" customWidth="1"/>
+    <col min="10" max="10" width="24.375" style="10" customWidth="1"/>
     <col min="11" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1556,7 +1564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1588,7 +1596,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1606,7 +1614,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -1638,7 +1646,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="34">
+    <row r="5" spans="1:10" ht="33" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1670,7 +1678,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>10101</v>
       </c>
@@ -1702,7 +1710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>10102</v>
       </c>
@@ -1734,7 +1742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>10103</v>
       </c>
@@ -1766,7 +1774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>10104</v>
       </c>
@@ -1798,7 +1806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>10105</v>
       </c>
@@ -1830,7 +1838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>10201</v>
       </c>
@@ -1860,7 +1868,7 @@
       </c>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>10202</v>
       </c>
@@ -1890,7 +1898,7 @@
       </c>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>10203</v>
       </c>
@@ -1921,7 +1929,7 @@
       <c r="J13" s="6"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="5" priority="75"/>
   </conditionalFormatting>
@@ -1933,68 +1941,91 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06B4D15F-7CDD-ED40-889B-A4868E886B80}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16">
+    <row r="1" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="16">
+      <c r="D1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="16">
+      <c r="D2" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="22"/>
-    </row>
-    <row r="4" spans="1:3" ht="16">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17">
+      <c r="D4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="22"/>
-    </row>
-    <row r="6" spans="1:3" ht="16">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -2004,8 +2035,14 @@
       <c r="C6" s="21" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="16">
+      <c r="D6" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>2</v>
       </c>
@@ -2015,8 +2052,10 @@
       <c r="C7" s="21" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="16">
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+    </row>
+    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>3</v>
       </c>
@@ -2026,8 +2065,10 @@
       <c r="C8" s="21" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="16">
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+    </row>
+    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>4</v>
       </c>
@@ -2037,15 +2078,19 @@
       <c r="C9" s="21" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="16">
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>5</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="21"/>
-    </row>
-    <row r="11" spans="1:3" ht="16">
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+    </row>
+    <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>6</v>
       </c>
@@ -2055,8 +2100,10 @@
       <c r="C11" s="21" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="16">
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+    </row>
+    <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>7</v>
       </c>
@@ -2066,8 +2113,10 @@
       <c r="C12" s="21" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="16">
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+    </row>
+    <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>8</v>
       </c>
@@ -2077,9 +2126,11 @@
       <c r="C13" s="21" t="s">
         <v>96</v>
       </c>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="A1:A13">
     <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
@@ -2091,23 +2142,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E27B46D-4699-4B1C-B2B1-8A327D06725E}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
     <col min="2" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="27" customFormat="1">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="26" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16">
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>118</v>
       </c>
@@ -2124,7 +2175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16">
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>103</v>
       </c>
@@ -2141,7 +2192,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16">
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -2152,7 +2203,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="16">
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2169,7 +2220,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16">
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2182,76 +2233,76 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16">
-      <c r="A7" s="25" t="s">
+    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="26">
-        <v>1</v>
-      </c>
-      <c r="D7" s="26">
-        <v>1</v>
-      </c>
-      <c r="E7" s="25" t="s">
+      <c r="C7" s="24">
+        <v>1</v>
+      </c>
+      <c r="D7" s="24">
+        <v>1</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16">
-      <c r="A8" s="25" t="s">
+    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C8" s="26">
-        <v>1</v>
-      </c>
-      <c r="D8" s="26">
+      <c r="C8" s="24">
+        <v>1</v>
+      </c>
+      <c r="D8" s="24">
         <v>2</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="23" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16">
-      <c r="A9" s="25" t="s">
+    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="24">
         <v>2</v>
       </c>
-      <c r="D9" s="26">
-        <v>1</v>
-      </c>
-      <c r="E9" s="25" t="s">
+      <c r="D9" s="24">
+        <v>1</v>
+      </c>
+      <c r="E9" s="23" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16">
-      <c r="A10" s="25" t="s">
+    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="24">
         <v>2</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="24">
         <v>2</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="23" t="s">
         <v>109</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="A2:A10">
     <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
@@ -2267,19 +2318,19 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
     <col min="2" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="27" customFormat="1">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="26" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16">
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2296,7 +2347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16">
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>103</v>
       </c>
@@ -2313,7 +2364,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16">
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -2324,7 +2375,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="16">
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2341,7 +2392,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16">
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2354,76 +2405,76 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16">
-      <c r="A7" s="25" t="s">
+    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="26">
-        <v>1</v>
-      </c>
-      <c r="D7" s="26">
-        <v>1</v>
-      </c>
-      <c r="E7" s="25" t="s">
+      <c r="C7" s="24">
+        <v>1</v>
+      </c>
+      <c r="D7" s="24">
+        <v>1</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16">
-      <c r="A8" s="25" t="s">
+    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C8" s="26">
-        <v>1</v>
-      </c>
-      <c r="D8" s="26">
+      <c r="C8" s="24">
+        <v>1</v>
+      </c>
+      <c r="D8" s="24">
         <v>2</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="23" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16">
-      <c r="A9" s="25" t="s">
+    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="24">
         <v>2</v>
       </c>
-      <c r="D9" s="26">
-        <v>1</v>
-      </c>
-      <c r="E9" s="25" t="s">
+      <c r="D9" s="24">
+        <v>1</v>
+      </c>
+      <c r="E9" s="23" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16">
-      <c r="A10" s="25" t="s">
+    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="24">
         <v>2</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="24">
         <v>2</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="23" t="s">
         <v>109</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="A2:A10">
     <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
@@ -2439,19 +2490,19 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
     <col min="2" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="27" customFormat="1">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="26" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16">
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2468,7 +2519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16">
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>103</v>
       </c>
@@ -2485,7 +2536,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16">
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -2496,7 +2547,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="16">
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2513,7 +2564,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16">
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2526,76 +2577,76 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16">
-      <c r="A7" s="25" t="s">
+    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="26">
-        <v>1</v>
-      </c>
-      <c r="D7" s="26">
-        <v>1</v>
-      </c>
-      <c r="E7" s="25" t="s">
+      <c r="C7" s="24">
+        <v>1</v>
+      </c>
+      <c r="D7" s="24">
+        <v>1</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16">
-      <c r="A8" s="25" t="s">
+    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C8" s="26">
-        <v>1</v>
-      </c>
-      <c r="D8" s="26">
+      <c r="C8" s="24">
+        <v>1</v>
+      </c>
+      <c r="D8" s="24">
         <v>2</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="23" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16">
-      <c r="A9" s="25" t="s">
+    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="24">
         <v>2</v>
       </c>
-      <c r="D9" s="26">
-        <v>1</v>
-      </c>
-      <c r="E9" s="25" t="s">
+      <c r="D9" s="24">
+        <v>1</v>
+      </c>
+      <c r="E9" s="23" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16">
-      <c r="A10" s="25" t="s">
+    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="24">
         <v>2</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="24">
         <v>2</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="23" t="s">
         <v>109</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="A2:A10">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
@@ -2611,19 +2662,19 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
     <col min="2" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="27" customFormat="1">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="26" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16">
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2640,7 +2691,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16">
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>103</v>
       </c>
@@ -2657,7 +2708,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16">
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -2668,7 +2719,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="16">
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2685,7 +2736,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16">
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2698,76 +2749,76 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16">
-      <c r="A7" s="25" t="s">
+    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="26">
-        <v>1</v>
-      </c>
-      <c r="D7" s="26">
-        <v>1</v>
-      </c>
-      <c r="E7" s="25" t="s">
+      <c r="C7" s="24">
+        <v>1</v>
+      </c>
+      <c r="D7" s="24">
+        <v>1</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16">
-      <c r="A8" s="25" t="s">
+    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C8" s="26">
-        <v>1</v>
-      </c>
-      <c r="D8" s="26">
+      <c r="C8" s="24">
+        <v>1</v>
+      </c>
+      <c r="D8" s="24">
         <v>2</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="23" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16">
-      <c r="A9" s="25" t="s">
+    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="24">
         <v>2</v>
       </c>
-      <c r="D9" s="26">
-        <v>1</v>
-      </c>
-      <c r="E9" s="25" t="s">
+      <c r="D9" s="24">
+        <v>1</v>
+      </c>
+      <c r="E9" s="23" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16">
-      <c r="A10" s="25" t="s">
+    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="24">
         <v>2</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="24">
         <v>2</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="23" t="s">
         <v>109</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="A2:A10">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
@@ -2783,15 +2834,15 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:2">
-      <c r="B2" s="24" t="s">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B2" s="22" t="s">
         <v>98</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>